<commit_message>
ver.0.3.9.1 végig kell tesztelni a adatok megadásától kezdve az excelbe írásig a át kell alakítani az excelt 150 sorosra, ha ok akkor mehet a 0.4.0
</commit_message>
<xml_diff>
--- a/2020-12__Tőke_Tamás_SFX-576_gkelsz.xlsx
+++ b/2020-12__Tőke_Tamás_SFX-576_gkelsz.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>ÚTNYILVÁNTARTÁS</t>
   </si>
@@ -128,10 +128,10 @@
     <t>SFX-576</t>
   </si>
   <si>
-    <t>8086</t>
-  </si>
-  <si>
-    <t>8741</t>
+    <t>8135</t>
+  </si>
+  <si>
+    <t>8570</t>
   </si>
   <si>
     <t xml:space="preserve"> Tőke Tamás</t>
@@ -143,7 +143,7 @@
     <t>6,7</t>
   </si>
   <si>
-    <t>0.0</t>
+    <t>12.6</t>
   </si>
   <si>
     <t>2020-12-01</t>
@@ -155,76 +155,25 @@
     <t>Székesfehérvár Udvardi utca 1/A</t>
   </si>
   <si>
-    <t>Veszprém Ady Endre u. 1.</t>
-  </si>
-  <si>
-    <t>CA38_ENA/UniCredit Bank Hungary Zrt.</t>
+    <t>Göd Ipartelep hrsz. 6901.</t>
+  </si>
+  <si>
+    <t>CA94/UniCredit Bank Hungary Zrt.</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>Veszprém Szeglethy u. 1.</t>
-  </si>
-  <si>
-    <t>CIB - ATM012/CIB Bank Zrt</t>
-  </si>
-  <si>
-    <t>Veszprém Egyetem ut 18</t>
-  </si>
-  <si>
-    <t>S6T73912/MTB Magyar Takarékszövetkezeti Bank</t>
-  </si>
-  <si>
     <t>telephely/telephely</t>
   </si>
   <si>
-    <t>2020-12-02</t>
-  </si>
-  <si>
-    <t>Mór Wekerle Sándor u. 34/a</t>
-  </si>
-  <si>
-    <t>AKHK2451/K &amp; H BANK ZRT.</t>
-  </si>
-  <si>
-    <t>Súr Petőfi u. 65.</t>
-  </si>
-  <si>
-    <t>S6T62904/MTB Magyar Takarékszövetkezeti Bank</t>
-  </si>
-  <si>
-    <t>2020-12-03</t>
-  </si>
-  <si>
-    <t>Lovasberény Rákóczi u. 1/a.</t>
-  </si>
-  <si>
-    <t>S6T73615/MTB Magyar Takarékszövetkezeti Bank</t>
-  </si>
-  <si>
-    <t>Siófok Fő út 186-188.</t>
-  </si>
-  <si>
-    <t>S02044/ERSTE BANK HUNGARY Zrt</t>
-  </si>
-  <si>
-    <t>Pázmánd Fő utca 87.</t>
-  </si>
-  <si>
-    <t>S6T57812/MTB Magyar Takarékszövetkezeti Bank</t>
-  </si>
-  <si>
-    <t>2020-12-04</t>
-  </si>
-  <si>
-    <t>Székesfehérvár Holland fasor 2.</t>
-  </si>
-  <si>
-    <t>DBD82220047/OTP BANK Nyrt.</t>
-  </si>
-  <si>
-    <t>2020-12-05</t>
+    <t>Siófok Fő tér 10/a</t>
+  </si>
+  <si>
+    <t>DBD82220009/OTP BANK Nyrt.</t>
+  </si>
+  <si>
+    <t>telephely</t>
   </si>
   <si>
     <t>Magán</t>
@@ -233,10 +182,13 @@
     <t>Magánhasználat</t>
   </si>
   <si>
-    <t>Nyíregyháza Hősök tere 7.</t>
-  </si>
-  <si>
-    <t>CIB - ATM007/CIB Bank Zrt</t>
+    <t>Székesfehérvár Takarodó ut 6</t>
+  </si>
+  <si>
+    <t>DPD DEPO/DPD</t>
+  </si>
+  <si>
+    <t>2020-12-18</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1140,7 @@
       </c>
       <c r="G5" s="8" t="str">
         <f>SUM(I10:I105)</f>
-        <v>1152</v>
+        <v>435</v>
       </c>
       <c r="J5" s="31"/>
     </row>
@@ -1205,7 +1157,7 @@
       </c>
       <c r="G6" s="9" t="str">
         <f>100*G7/G5</f>
-        <v/>
+        <v>2.896</v>
       </c>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
@@ -1298,13 +1250,13 @@
       </c>
       <c r="G10" s="26" t="n">
         <f>IF(B10&lt;&gt;"",$C$5+I10,"")</f>
-        <v>8135.0</v>
+        <v>8225.0</v>
       </c>
       <c r="H10" s="21" t="n">
         <v>0.0</v>
       </c>
       <c r="I10" s="21" t="n">
-        <v>49.0</v>
+        <v>90.0</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>42</v>
@@ -1324,20 +1276,20 @@
         <v>40</v>
       </c>
       <c r="E11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="21" t="s">
         <v>43</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>44</v>
       </c>
       <c r="G11" s="26" t="n">
         <f>IF(B11&lt;&gt;"",G10+I11,"")</f>
-        <v>8136.0</v>
+        <v>8315.0</v>
       </c>
       <c r="H11" s="21" t="n">
         <v>0.0</v>
       </c>
       <c r="I11" s="21" t="n">
-        <v>1.0</v>
+        <v>90.0</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>42</v>
@@ -1354,23 +1306,23 @@
         <v>38</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E12" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>45</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>46</v>
       </c>
       <c r="G12" s="26" t="n">
         <f t="shared" ref="G12:G54" si="0">IF(B12&lt;&gt;"",G11+I12,"")</f>
-        <v>8137.0</v>
+        <v>8367.0</v>
       </c>
       <c r="H12" s="21" t="n">
         <v>0.0</v>
       </c>
       <c r="I12" s="21" t="n">
-        <v>1.0</v>
+        <v>52.0</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>42</v>
@@ -1390,23 +1342,23 @@
         <v>38</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>39</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" s="26" t="n">
         <f t="shared" si="0"/>
-        <v>8188.0</v>
+        <v>8419.0</v>
       </c>
       <c r="H13" s="21" t="n">
-        <v>0.0</v>
+        <v>12.6</v>
       </c>
       <c r="I13" s="21" t="n">
-        <v>51.0</v>
+        <v>52.0</v>
       </c>
       <c r="J13" s="19" t="s">
         <v>42</v>
@@ -1420,32 +1372,32 @@
         <v>5</v>
       </c>
       <c r="B14" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>39</v>
-      </c>
       <c r="E14" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G14" s="26" t="n">
         <f t="shared" si="0"/>
-        <v>8219.0</v>
+        <v>8542.0</v>
       </c>
       <c r="H14" s="21" t="n">
         <v>0.0</v>
       </c>
       <c r="I14" s="21" t="n">
-        <v>31.0</v>
+        <v>123.0</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1453,29 +1405,29 @@
         <v>6</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>51</v>
-      </c>
       <c r="F15" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G15" s="26" t="n">
         <f t="shared" si="0"/>
-        <v>8241.0</v>
+        <v>8550.0</v>
       </c>
       <c r="H15" s="21" t="n">
         <v>0.0</v>
       </c>
       <c r="I15" s="21" t="n">
-        <v>22.0</v>
+        <v>8.0</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>42</v>
@@ -1486,29 +1438,29 @@
         <v>7</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G16" s="26" t="n">
         <f t="shared" si="0"/>
-        <v>8288.0</v>
+        <v>8558.0</v>
       </c>
       <c r="H16" s="21" t="n">
         <v>0.0</v>
       </c>
       <c r="I16" s="21" t="n">
-        <v>47.0</v>
+        <v>8.0</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>42</v>
@@ -1519,297 +1471,169 @@
         <v>8</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G17" s="26" t="n">
         <f t="shared" si="0"/>
-        <v>8304.0</v>
+        <v>8570.0</v>
       </c>
       <c r="H17" s="21" t="n">
         <v>0.0</v>
       </c>
       <c r="I17" s="21" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>9</v>
       </c>
-      <c r="B18" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="26" t="n">
-        <f t="shared" si="0"/>
-        <v>8371.0</v>
-      </c>
-      <c r="H18" s="21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I18" s="21" t="n">
-        <v>67.0</v>
-      </c>
-      <c r="J18" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="19"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>10</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="26" t="n">
-        <f t="shared" si="0"/>
-        <v>8439.0</v>
-      </c>
-      <c r="H19" s="21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I19" s="21" t="n">
-        <v>68.0</v>
-      </c>
-      <c r="J19" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>12</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="26" t="n">
-        <f t="shared" si="0"/>
-        <v>8461.0</v>
-      </c>
-      <c r="H20" s="21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I20" s="21" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="19"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>13</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="26" t="n">
-        <f t="shared" si="0"/>
-        <v>8473.0</v>
-      </c>
-      <c r="H21" s="21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I21" s="21" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="J21" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="19"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>14</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="26" t="n">
-        <f t="shared" si="0"/>
-        <v>8485.0</v>
-      </c>
-      <c r="H22" s="21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I22" s="21" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="J22" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="19"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>15</v>
       </c>
-      <c r="B23" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" s="26" t="n">
-        <f t="shared" si="0"/>
-        <v>8612.0</v>
-      </c>
-      <c r="H23" s="21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I23" s="21" t="n">
-        <v>127.0</v>
-      </c>
-      <c r="J23" s="19" t="s">
-        <v>23</v>
-      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="19"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>16</v>
       </c>
-      <c r="B24" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="26" t="n">
-        <f t="shared" si="0"/>
-        <v>8925.0</v>
-      </c>
-      <c r="H24" s="21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I24" s="21" t="n">
-        <v>313.0</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>17</v>
       </c>
-      <c r="B25" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" s="26" t="n">
-        <f t="shared" si="0"/>
-        <v>9238.0</v>
-      </c>
-      <c r="H25" s="21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I25" s="21" t="n">
-        <v>313.0</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="19"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
@@ -3141,7 +2965,7 @@
       </c>
       <c r="L103" s="35" t="str">
         <f>SUM(I10:I105)</f>
-        <v>1152</v>
+        <v>435</v>
       </c>
       <c r="M103" s="36"/>
     </row>
@@ -3166,11 +2990,11 @@
       </c>
       <c r="L104" s="38" t="str">
         <f>SUMIF(J10:J105,"M",I10:I105)</f>
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="M104" s="39" t="str">
         <f>L104/L103</f>
-        <v>11%</v>
+        <v>31%</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -3194,7 +3018,7 @@
       </c>
       <c r="L105" s="41" t="str">
         <f>C5+L103</f>
-        <v>8741</v>
+        <v>8570</v>
       </c>
       <c r="M105" s="42"/>
     </row>

</xml_diff>